<commit_message>
major additions to housekeeping UI
</commit_message>
<xml_diff>
--- a/lib/SAILFormat.xlsx
+++ b/lib/SAILFormat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\Sailproj\SailProjGit\SAILcode\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B019D438-988A-47BF-95B4-867B383ABFFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51924AF5-C48B-46F8-A653-0A3D27E0840C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="59">
   <si>
     <t>Graph #</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Start Row</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -691,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -921,6 +924,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1246,18 +1252,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7758D255-7225-412E-BCCB-5D6A66A51808}">
-  <dimension ref="A2:U34"/>
+  <dimension ref="A2:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="11" width="16.7109375" customWidth="1"/>
-    <col min="12" max="22" width="15.5703125" customWidth="1"/>
+    <col min="2" max="22" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
@@ -1573,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B17" s="84"/>
       <c r="C17" s="29">
         <v>4</v>
@@ -1615,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="84"/>
       <c r="C18" s="30">
         <v>4</v>
@@ -1657,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B19" s="84" t="s">
         <v>32</v>
       </c>
@@ -1701,7 +1705,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B20" s="84"/>
       <c r="C20" s="29">
         <v>0</v>
@@ -1743,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="84"/>
       <c r="C21" s="45">
         <v>1</v>
@@ -1785,7 +1789,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B22" s="85" t="s">
         <v>33</v>
       </c>
@@ -1829,7 +1833,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B23" s="86"/>
       <c r="C23" s="29">
         <v>2</v>
@@ -1871,7 +1875,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="86"/>
       <c r="C24" s="30">
         <v>2</v>
@@ -1913,7 +1917,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B25" s="87"/>
       <c r="C25" s="28">
         <v>3</v>
@@ -1955,7 +1959,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="87"/>
       <c r="C26" s="29">
@@ -1998,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="82"/>
       <c r="C27" s="29">
@@ -2041,7 +2045,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B28" s="81" t="s">
         <v>18</v>
       </c>
@@ -2085,7 +2089,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B29" s="82"/>
       <c r="C29" s="29">
         <v>5</v>
@@ -2127,112 +2131,114 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="68" t="s">
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="69" t="s">
+      <c r="E31" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="E31" s="69" t="s">
+      <c r="F31" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="69" t="s">
+      <c r="G31" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="69" t="s">
+      <c r="H31" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="H31" s="70" t="s">
+      <c r="I31" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="I31" s="70" t="s">
+      <c r="J31" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="J31" s="71" t="s">
+      <c r="K31" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="K31" s="60" t="s">
+      <c r="L31" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="L31" s="61" t="s">
+      <c r="M31" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="M31" s="61" t="s">
+      <c r="N31" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="N31" s="61" t="s">
+      <c r="O31" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="O31" s="61" t="s">
+      <c r="P31" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="P31" s="62" t="s">
+      <c r="Q31" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="Q31" s="62" t="s">
+      <c r="R31" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="R31" s="62" t="s">
+      <c r="S31" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="S31" s="62" t="s">
+      <c r="T31" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="T31" s="75" t="s">
+      <c r="U31" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="U31" s="63" t="s">
+      <c r="V31" s="63" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B32" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="72" t="s">
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="67">
+      <c r="E32" s="67">
         <v>135</v>
       </c>
-      <c r="E32" s="67">
+      <c r="F32" s="67">
         <v>11</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G32" s="1">
+      <c r="H32" s="1">
         <v>12500</v>
       </c>
-      <c r="H32" s="54">
+      <c r="I32" s="54">
         <v>39</v>
       </c>
-      <c r="I32" s="54">
+      <c r="J32" s="54">
         <v>15</v>
       </c>
-      <c r="J32" s="55">
+      <c r="K32" s="55">
         <v>0</v>
       </c>
-      <c r="K32" s="64" t="b">
+      <c r="L32" s="64" t="b">
         <f>TRUE()</f>
         <v>1</v>
-      </c>
-      <c r="L32" s="59" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
       </c>
       <c r="M32" s="59" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="N32" s="59" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="O32" s="59" t="b">
         <f>TRUE()</f>
@@ -2254,131 +2260,137 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T32" s="76" t="b">
+      <c r="T32" s="59" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U32" s="78" t="b">
+      <c r="U32" s="76" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="V32" s="78" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="1">
+        <v>18</v>
+      </c>
+      <c r="F33" s="67">
+        <v>11</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H33" s="1">
+        <v>25000</v>
+      </c>
+      <c r="I33" s="54">
+        <v>21</v>
+      </c>
+      <c r="J33" s="54">
+        <v>255</v>
+      </c>
+      <c r="K33" s="55">
+        <v>0</v>
+      </c>
+      <c r="L33" s="64" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M33" s="59" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N33" s="59" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B33" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="72" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="1">
-        <v>18</v>
-      </c>
-      <c r="E33" s="67">
-        <v>11</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" s="1">
-        <v>25000</v>
-      </c>
-      <c r="H33" s="54">
-        <v>21</v>
-      </c>
-      <c r="I33" s="54">
-        <v>255</v>
-      </c>
-      <c r="J33" s="55">
-        <v>0</v>
-      </c>
-      <c r="K33" s="64" t="b">
+      <c r="O33" s="59" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L33" s="59" t="b">
+      <c r="P33" s="59" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M33" s="59" t="b">
+      <c r="Q33" s="59" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R33" s="59" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S33" s="59" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="T33" s="59" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U33" s="76" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="V33" s="78" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="N33" s="59" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O33" s="59" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="P33" s="59" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="Q33" s="59" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R33" s="59" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="S33" s="59" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="T33" s="76" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U33" s="78" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="73" t="s">
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="74">
+      <c r="E34" s="74">
         <v>51</v>
       </c>
-      <c r="E34" s="74">
+      <c r="F34" s="74">
         <v>11</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="G34" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="7">
+      <c r="H34" s="7">
         <v>25000</v>
       </c>
-      <c r="H34" s="56">
+      <c r="I34" s="56">
         <v>63</v>
       </c>
-      <c r="I34" s="56">
-        <v>255</v>
-      </c>
-      <c r="J34" s="57">
+      <c r="J34" s="56">
+        <v>255</v>
+      </c>
+      <c r="K34" s="57">
         <v>0</v>
       </c>
-      <c r="K34" s="65" t="b">
+      <c r="L34" s="65" t="b">
         <f>TRUE()</f>
         <v>1</v>
-      </c>
-      <c r="L34" s="66" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
       </c>
       <c r="M34" s="66" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="N34" s="66" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="O34" s="66" t="b">
         <f>TRUE()</f>
@@ -2400,14 +2412,21 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T34" s="77" t="b">
+      <c r="T34" s="66" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U34" s="79" t="b">
+      <c r="U34" s="77" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="V34" s="79" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E43" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2422,7 +2441,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="M32:M34 L33" formula="1"/>
+    <ignoredError sqref="N32:N34 M33" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Started on plotting ui
</commit_message>
<xml_diff>
--- a/lib/SAILFormat.xlsx
+++ b/lib/SAILFormat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\Sailproj\SailProjGit\SAILcode\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E72710-753E-49FD-A2BC-35A60DEA9D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B978DA6E-2061-4A45-BB6D-26D177002986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
   </bookViews>
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7758D255-7225-412E-BCCB-5D6A66A51808}">
   <dimension ref="A2:V43"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="C9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
House keeping values work
</commit_message>
<xml_diff>
--- a/lib/SAILFormat.xlsx
+++ b/lib/SAILFormat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\Sailproj\SailProjGit\SAILcode\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B978DA6E-2061-4A45-BB6D-26D177002986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37F14AF-6CE6-4BC9-ACB7-3F68441DEACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
   </bookViews>
@@ -901,6 +901,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -924,9 +927,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7758D255-7225-412E-BCCB-5D6A66A51808}">
   <dimension ref="A2:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="C9:H9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,16 +1322,16 @@
       <c r="F7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="83" t="s">
+      <c r="G7" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="83"/>
+      <c r="H7" s="84"/>
       <c r="I7" s="39" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="81" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -1359,7 +1359,7 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="80"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="14" t="s">
         <v>12</v>
       </c>
@@ -1385,7 +1385,7 @@
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="80"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="14" t="s">
         <v>13</v>
       </c>
@@ -1411,7 +1411,7 @@
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="80"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="14" t="s">
         <v>17</v>
       </c>
@@ -1437,7 +1437,7 @@
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="80"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="14" t="s">
         <v>10</v>
       </c>
@@ -1463,7 +1463,7 @@
       </c>
     </row>
     <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="80"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="16" t="s">
         <v>18</v>
       </c>
@@ -1533,8 +1533,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="84" t="s">
+    <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="85" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="28">
@@ -1546,7 +1546,8 @@
       <c r="E16" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="25" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G16" s="21">
@@ -1577,8 +1578,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="84"/>
+    <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="85"/>
       <c r="C17" s="29">
         <v>4</v>
       </c>
@@ -1588,7 +1589,8 @@
       <c r="E17" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="25" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G17" s="2">
@@ -1620,7 +1622,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="84"/>
+      <c r="B18" s="85"/>
       <c r="C18" s="30">
         <v>4</v>
       </c>
@@ -1630,7 +1632,8 @@
       <c r="E18" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="25" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G18" s="8">
@@ -1661,8 +1664,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="84" t="s">
+    <row r="19" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="85" t="s">
         <v>32</v>
       </c>
       <c r="C19" s="28">
@@ -1674,7 +1677,8 @@
       <c r="E19" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="25" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G19" s="21">
@@ -1705,8 +1709,8 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="84"/>
+    <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="85"/>
       <c r="C20" s="29">
         <v>0</v>
       </c>
@@ -1716,7 +1720,8 @@
       <c r="E20" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="25" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G20" s="2">
@@ -1748,7 +1753,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="84"/>
+      <c r="B21" s="85"/>
       <c r="C21" s="45">
         <v>1</v>
       </c>
@@ -1758,7 +1763,8 @@
       <c r="E21" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="47">
+      <c r="F21" s="25" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G21" s="48">
@@ -1789,8 +1795,8 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="85" t="s">
+    <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="86" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="28">
@@ -1802,7 +1808,8 @@
       <c r="E22" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="25" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G22" s="21">
@@ -1833,8 +1840,8 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="86"/>
+    <row r="23" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="87"/>
       <c r="C23" s="29">
         <v>2</v>
       </c>
@@ -1844,7 +1851,8 @@
       <c r="E23" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="26">
+      <c r="F23" s="25" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G23" s="2">
@@ -1876,7 +1884,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="86"/>
+      <c r="B24" s="87"/>
       <c r="C24" s="30">
         <v>2</v>
       </c>
@@ -1886,7 +1894,8 @@
       <c r="E24" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="25" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G24" s="8">
@@ -1917,8 +1926,8 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="87"/>
+    <row r="25" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="88"/>
       <c r="C25" s="28">
         <v>3</v>
       </c>
@@ -1928,7 +1937,8 @@
       <c r="E25" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="25" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G25" s="21">
@@ -1959,9 +1969,9 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
-      <c r="B26" s="87"/>
+      <c r="B26" s="88"/>
       <c r="C26" s="29">
         <v>3</v>
       </c>
@@ -1971,7 +1981,8 @@
       <c r="E26" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="25" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G26" s="2">
@@ -2004,7 +2015,7 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
-      <c r="B27" s="82"/>
+      <c r="B27" s="83"/>
       <c r="C27" s="29">
         <v>3</v>
       </c>
@@ -2014,7 +2025,8 @@
       <c r="E27" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="26">
+      <c r="F27" s="25" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="G27" s="2">
@@ -2046,7 +2058,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B28" s="81" t="s">
+      <c r="B28" s="82" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="52">
@@ -2058,7 +2070,8 @@
       <c r="E28" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="F28" s="41">
+      <c r="F28" s="41" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="G28" s="42">
@@ -2090,7 +2103,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B29" s="82"/>
+      <c r="B29" s="83"/>
       <c r="C29" s="29">
         <v>5</v>
       </c>
@@ -2100,7 +2113,8 @@
       <c r="E29" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="26">
+      <c r="F29" s="41" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="G29" s="2">
@@ -2241,8 +2255,8 @@
         <v>0</v>
       </c>
       <c r="O32" s="59" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="P32" s="59" t="b">
         <f>TRUE()</f>
@@ -2317,8 +2331,8 @@
         <v>0</v>
       </c>
       <c r="O33" s="59" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="P33" s="59" t="b">
         <f>TRUE()</f>
@@ -2426,7 +2440,7 @@
       </c>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="E43" s="88"/>
+      <c r="E43" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2447,6 +2461,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085EDC4FCBFEAC44C90B472F1F1C900EA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e45273375250329c822a0a405177b348">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xmlns:ns4="6b4e13fc-0909-4af8-88c8-1f82cb55b253" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0e1ca657407e685f067414fb59c7721" ns3:_="" ns4:_="">
     <xsd:import namespace="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
@@ -2675,38 +2706,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917E079B-BC71-4494-9E92-79C803C2F6BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
-    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2729,9 +2732,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917E079B-BC71-4494-9E92-79C803C2F6BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
+    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>